<commit_message>
fixed col detection failure; BS line item classification failure
</commit_message>
<xml_diff>
--- a/LOGS/26cd4795-4ed5-49af-a3d7-5dc6826a64bc/main_page_service_output/main_pages.xlsx
+++ b/LOGS/26cd4795-4ed5-49af-a3d7-5dc6826a64bc/main_page_service_output/main_pages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="96">
   <si>
     <t>Particulars</t>
   </si>
@@ -237,7 +237,73 @@
     <t>6</t>
   </si>
   <si>
+    <t>Cash flows from operating activities</t>
+  </si>
+  <si>
+    <t>Receipts from customers (inclusive of goods and services tax)</t>
+  </si>
+  <si>
+    <t>Payments to suppliers and employees (inclusive of goods and services</t>
+  </si>
+  <si>
+    <t>tax)</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>Interest received</t>
+  </si>
+  <si>
+    <t>Interest paid</t>
+  </si>
+  <si>
+    <t>Income taxes paid</t>
+  </si>
+  <si>
+    <t>Net cash inflow (outflow) from operating activities</t>
+  </si>
+  <si>
+    <t>Cash flows from investing activities</t>
+  </si>
+  <si>
+    <t>Payments for property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Net cash (outflow) from investing activities</t>
+  </si>
+  <si>
+    <t>Cash flows from financing activities</t>
+  </si>
+  <si>
+    <t>Principal elements of lease payments</t>
+  </si>
+  <si>
+    <t>Net cash (outflow) from financing activities</t>
+  </si>
+  <si>
+    <t>Net increase (decrease) in cash and cash equivalents</t>
+  </si>
+  <si>
+    <t>Cash and cash equivalents at the beginning of the financial year</t>
+  </si>
+  <si>
+    <t>Effects of exchange rate changes on cash and cash equivalents</t>
+  </si>
+  <si>
     <t>Cash and cash equivalents at end of year</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>operating_activities</t>
+  </si>
+  <si>
+    <t>investing_activities</t>
+  </si>
+  <si>
+    <t>financing_activities</t>
   </si>
 </sst>
 </file>
@@ -595,7 +661,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -860,10 +926,10 @@
         <v>41513852</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1062,7 +1128,7 @@
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1079,7 +1145,7 @@
         <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1173,6 +1239,592 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="C32">
+        <v>2023</v>
+      </c>
+      <c r="D32">
+        <v>2022</v>
+      </c>
+      <c r="E32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>13525659</v>
+      </c>
+      <c r="E36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>6065110</v>
+      </c>
+      <c r="D37">
+        <v>5021477</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <v>20980853</v>
+      </c>
+      <c r="D38">
+        <v>21454750</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39">
+        <v>2073287</v>
+      </c>
+      <c r="D39">
+        <v>1358477</v>
+      </c>
+      <c r="E39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>45990769</v>
+      </c>
+      <c r="D40">
+        <v>41360363</v>
+      </c>
+      <c r="E40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42">
+        <v>8569</v>
+      </c>
+      <c r="D42">
+        <v>10748</v>
+      </c>
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43">
+        <v>105724</v>
+      </c>
+      <c r="D43">
+        <v>109331</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44">
+        <v>34261</v>
+      </c>
+      <c r="D44">
+        <v>33410</v>
+      </c>
+      <c r="E44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45">
+        <v>148554</v>
+      </c>
+      <c r="D45">
+        <v>153489</v>
+      </c>
+      <c r="E45" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46">
+        <v>46139323</v>
+      </c>
+      <c r="D46">
+        <v>41513852</v>
+      </c>
+      <c r="E46" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49">
+        <v>9502391</v>
+      </c>
+      <c r="D49">
+        <v>9636475</v>
+      </c>
+      <c r="E49" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50">
+        <v>57712</v>
+      </c>
+      <c r="D50">
+        <v>79066</v>
+      </c>
+      <c r="E50" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51">
+        <v>340279</v>
+      </c>
+      <c r="D51">
+        <v>247279</v>
+      </c>
+      <c r="E51" t="s">
+        <v>47</v>
+      </c>
+      <c r="F51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52">
+        <v>54862</v>
+      </c>
+      <c r="D52">
+        <v>48150</v>
+      </c>
+      <c r="E52" t="s">
+        <v>47</v>
+      </c>
+      <c r="F52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53">
+        <v>9955244</v>
+      </c>
+      <c r="D53">
+        <v>10010970</v>
+      </c>
+      <c r="E53" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>47</v>
+      </c>
+      <c r="F54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55">
+        <v>49009</v>
+      </c>
+      <c r="D55">
+        <v>28411</v>
+      </c>
+      <c r="E55" t="s">
+        <v>47</v>
+      </c>
+      <c r="F55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56">
+        <v>49009</v>
+      </c>
+      <c r="D56">
+        <v>28411</v>
+      </c>
+      <c r="E56" t="s">
+        <v>47</v>
+      </c>
+      <c r="F56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <v>10004253</v>
+      </c>
+      <c r="D57">
+        <v>10039381</v>
+      </c>
+      <c r="E57" t="s">
+        <v>47</v>
+      </c>
+      <c r="F57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58">
+        <v>36135070</v>
+      </c>
+      <c r="D58">
+        <v>31474471</v>
+      </c>
+      <c r="E58" t="s">
+        <v>47</v>
+      </c>
+      <c r="F58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F59" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60">
+        <v>25467389</v>
+      </c>
+      <c r="D60">
+        <v>25467389</v>
+      </c>
+      <c r="E60" t="s">
+        <v>47</v>
+      </c>
+      <c r="F60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61">
+        <v>1945682</v>
+      </c>
+      <c r="D61">
+        <v>-1255697</v>
+      </c>
+      <c r="E61" t="s">
+        <v>47</v>
+      </c>
+      <c r="F61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62">
+        <v>8721999</v>
+      </c>
+      <c r="D62">
+        <v>7262779</v>
+      </c>
+      <c r="E62" t="s">
+        <v>47</v>
+      </c>
+      <c r="F62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63">
+        <v>36135070</v>
+      </c>
+      <c r="D63">
+        <v>31474471</v>
+      </c>
+      <c r="E63" t="s">
+        <v>47</v>
+      </c>
+      <c r="F63" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1183,7 +1835,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1416,6 +2068,238 @@
         <v>1463607</v>
       </c>
     </row>
+    <row r="20" spans="1:4">
+      <c r="C20">
+        <v>2023</v>
+      </c>
+      <c r="D20">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>122961155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24">
+        <v>453175</v>
+      </c>
+      <c r="D24">
+        <v>697369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="C25">
+        <v>157162456</v>
+      </c>
+      <c r="D25">
+        <v>123658524</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>-36252</v>
+      </c>
+      <c r="D26">
+        <v>-67214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28">
+        <v>-151263638</v>
+      </c>
+      <c r="D28">
+        <v>-119142037</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29">
+        <v>-114428</v>
+      </c>
+      <c r="D29">
+        <v>-107467</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30">
+        <v>-63887</v>
+      </c>
+      <c r="D30">
+        <v>-101558</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31">
+        <v>-510266</v>
+      </c>
+      <c r="D31">
+        <v>-396461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>-3312669</v>
+      </c>
+      <c r="D32">
+        <v>-2534370</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33">
+        <v>-2844</v>
+      </c>
+      <c r="D33">
+        <v>-2516</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34">
+        <v>1858472</v>
+      </c>
+      <c r="D34">
+        <v>1306901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35">
+        <v>-399252</v>
+      </c>
+      <c r="D35">
+        <v>-261394</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36">
+        <v>1459220</v>
+      </c>
+      <c r="D36">
+        <v>1045507</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>3201379</v>
+      </c>
+      <c r="D38">
+        <v>418100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <v>4660599</v>
+      </c>
+      <c r="D39">
+        <v>1463607</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1423,38 +2307,299 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
         <v>2023</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>2022</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>73</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3">
+        <v>155346538</v>
+      </c>
+      <c r="D3">
+        <v>125024684</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>-154805634</v>
+      </c>
+      <c r="D5">
+        <v>-128338226</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>540904</v>
+      </c>
+      <c r="D6">
+        <v>-3313542</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7">
+        <v>57475</v>
+      </c>
+      <c r="D7">
+        <v>3746</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8">
+        <v>-47484</v>
+      </c>
+      <c r="D8">
+        <v>-47142</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>-307103</v>
+      </c>
+      <c r="D9">
+        <v>-236502</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10">
+        <v>243792</v>
+      </c>
+      <c r="D10">
+        <v>-3593440</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12">
+        <v>-4876</v>
+      </c>
+      <c r="D12">
+        <v>-3384</v>
+      </c>
+      <c r="E12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13">
+        <v>-4876</v>
+      </c>
+      <c r="D13">
+        <v>-3384</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15">
+        <v>-94435</v>
+      </c>
+      <c r="D15">
+        <v>-40778</v>
+      </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16">
+        <v>-94435</v>
+      </c>
+      <c r="D16">
+        <v>-40778</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17">
+        <v>144481</v>
+      </c>
+      <c r="D17">
+        <v>-3637602</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18">
+        <v>13525659</v>
+      </c>
+      <c r="D18">
+        <v>16745161</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19">
+        <v>3201379</v>
+      </c>
+      <c r="D19">
+        <v>418100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20">
+        <v>16871519</v>
+      </c>
+      <c r="D20">
+        <v>13525659</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>